<commit_message>
Marketing Plan checked in
Marketing Plan checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/MarketingMasterPlan-May-2023.xlsx
+++ b/Offline/BusinessManagement/Marketing/MarketingMasterPlan-May-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DA6B2E-89FC-452A-ABA5-83B1F3C3B860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B05A3B-ADD8-4BE8-BF05-7D2D0F54170B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="836" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="836" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MarketingRatingSheet" sheetId="13" r:id="rId1"/>
@@ -24,11 +24,12 @@
     <sheet name="Generic" sheetId="17" r:id="rId9"/>
     <sheet name="Artworks" sheetId="12" r:id="rId10"/>
     <sheet name="RoadShows" sheetId="23" r:id="rId11"/>
-    <sheet name="MarketingPlan" sheetId="14" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="18" r:id="rId13"/>
+    <sheet name="Sheet2" sheetId="24" r:id="rId12"/>
+    <sheet name="MarketingPlan" sheetId="14" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">MarketingPlan!$N$1:$P$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">MarketingPlan!$N$1:$P$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="635">
   <si>
     <t>Medium</t>
   </si>
@@ -1940,6 +1941,30 @@
   </si>
   <si>
     <t>Woodsquare Mall</t>
+  </si>
+  <si>
+    <t>CRM Followup</t>
+  </si>
+  <si>
+    <t>RSVP of Seminars</t>
+  </si>
+  <si>
+    <t>Deliver Seminars</t>
+  </si>
+  <si>
+    <t>Teacher's Profile</t>
+  </si>
+  <si>
+    <t>Course Fees</t>
+  </si>
+  <si>
+    <t>Seminar PPTs  --&gt; All Swimlanes</t>
+  </si>
+  <si>
+    <t>Visit Sheets (Pre CRM)</t>
+  </si>
+  <si>
+    <t>Misc</t>
   </si>
 </sst>
 </file>
@@ -6881,8 +6906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915E635A-68CA-4147-811F-424EF28651FA}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7114,6 +7139,64 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE84DDF1-DEE0-4E2B-8321-6AA75B5475A2}">
+  <dimension ref="B2:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>634</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P83"/>
   <sheetViews>
@@ -8084,7 +8167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C788D979-7CB4-4DA8-AE6B-ABB33AE1CBEA}">
   <dimension ref="A1:J68"/>
   <sheetViews>

</xml_diff>